<commit_message>
Added Internal Location structure
</commit_message>
<xml_diff>
--- a/System Analysis/WorkingRepository/Group4/SUBSET_26_3-6/Spread-sheet-SUBSET_26-2-6_Train-Position-Information.xlsx
+++ b/System Analysis/WorkingRepository/Group4/SUBSET_26_3-6/Spread-sheet-SUBSET_26-2-6_Train-Position-Information.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="149">
   <si>
     <t>Template for System Analysis</t>
   </si>
@@ -547,6 +547,12 @@
   </si>
   <si>
     <t>Gives Object specific data as a structure (specific for all track objects)</t>
+  </si>
+  <si>
+    <t>nominalLocation</t>
+  </si>
+  <si>
+    <t>Absolute Position on the trip</t>
   </si>
 </sst>
 </file>
@@ -903,6 +909,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -919,24 +934,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -957,8 +954,17 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1323,15 +1329,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" ht="15.75">
       <c r="A2" s="1"/>
@@ -1439,13 +1445,13 @@
       <c r="A27" s="4"/>
     </row>
     <row r="28" spans="1:5" ht="66.75" customHeight="1">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
     </row>
     <row r="29" spans="1:5" ht="15.75">
       <c r="A29" s="1"/>
@@ -1534,16 +1540,16 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="31" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="11" t="s">
@@ -1558,18 +1564,18 @@
       <c r="H2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="31" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="27"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="32"/>
       <c r="E3" s="11" t="s">
         <v>26</v>
       </c>
@@ -1582,8 +1588,8 @@
       <c r="H3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="75">
       <c r="A4" s="23" t="s">
@@ -2305,28 +2311,28 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="31" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="31" t="s">
         <v>25</v>
       </c>
       <c r="I2" s="12" t="s">
@@ -2334,31 +2340,31 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
       <c r="C3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
       <c r="I3" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9">
@@ -2533,8 +2539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2544,73 +2550,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="41" t="s">
         <v>37</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="41" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
       <c r="H2" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
     </row>
     <row r="3" spans="1:12" ht="31.5">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="31" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="31" t="s">
         <v>23</v>
       </c>
       <c r="F3" s="10" t="s">
@@ -2625,24 +2631,24 @@
       <c r="I3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="J3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="31" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
       <c r="F4" s="10" t="s">
         <v>26</v>
       </c>
@@ -2655,210 +2661,216 @@
       <c r="I4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-    </row>
-    <row r="5" spans="1:12" s="36" customFormat="1" ht="15.75">
-      <c r="A5" s="41" t="s">
+      <c r="J4" s="34"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+    </row>
+    <row r="5" spans="1:12" s="26" customFormat="1" ht="15.75">
+      <c r="A5" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="43"/>
-    </row>
-    <row r="6" spans="1:12" s="36" customFormat="1" ht="30">
-      <c r="A6" s="34" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="40"/>
+    </row>
+    <row r="6" spans="1:12" s="26" customFormat="1" ht="30">
+      <c r="A6" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34" t="s">
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="K6" s="34"/>
-      <c r="L6" s="44" t="s">
+      <c r="K6" s="24"/>
+      <c r="L6" s="28" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="36" customFormat="1" ht="15.75">
-      <c r="A7" s="37" t="s">
+    <row r="7" spans="1:12" s="26" customFormat="1" ht="15.75">
+      <c r="A7" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="36" customFormat="1" ht="31.5">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:12" s="26" customFormat="1" ht="31.5">
+      <c r="A8" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37" t="s">
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="36" customFormat="1" ht="31.5">
-      <c r="A9" s="37" t="s">
+    <row r="9" spans="1:12" s="26" customFormat="1" ht="31.5">
+      <c r="A9" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37" t="s">
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37" t="s">
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="36" customFormat="1" ht="31.5">
-      <c r="A10" s="37" t="s">
+    <row r="10" spans="1:12" s="26" customFormat="1" ht="31.5">
+      <c r="A10" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37" t="s">
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37" t="s">
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="36" customFormat="1" ht="31.5">
-      <c r="A11" s="37" t="s">
+    <row r="11" spans="1:12" s="26" customFormat="1" ht="31.5">
+      <c r="A11" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37" t="s">
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37" t="s">
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="36" customFormat="1" ht="15.75">
-      <c r="A12" s="37"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
-    </row>
-    <row r="13" spans="1:12" s="36" customFormat="1" ht="15.75">
-      <c r="A13" s="38" t="s">
+    <row r="12" spans="1:12" s="26" customFormat="1" ht="15.75">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+    </row>
+    <row r="13" spans="1:12" s="26" customFormat="1" ht="15.75">
+      <c r="A13" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="40"/>
-    </row>
-    <row r="14" spans="1:12" s="35" customFormat="1">
-      <c r="A14" s="34" t="s">
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="37"/>
+    </row>
+    <row r="14" spans="1:12" s="25" customFormat="1">
+      <c r="A14" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="14"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75">
+      <c r="A15" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75">
+      <c r="A16" s="27" t="s">
+        <v>147</v>
+      </c>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
@@ -2869,35 +2881,49 @@
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
+      <c r="L16" s="27" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="31.5">
+      <c r="A17" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="31.5">
+      <c r="A18" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="14"/>
@@ -2941,21 +2967,21 @@
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
     </row>
-    <row r="22" spans="1:12" s="35" customFormat="1">
-      <c r="A22" s="34" t="s">
+    <row r="22" spans="1:12" s="25" customFormat="1">
+      <c r="A22" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="14"/>
@@ -3027,21 +3053,21 @@
       <c r="K27" s="14"/>
       <c r="L27" s="14"/>
     </row>
-    <row r="28" spans="1:12" s="35" customFormat="1">
-      <c r="A28" s="34" t="s">
+    <row r="28" spans="1:12" s="25" customFormat="1">
+      <c r="A28" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="14"/>
@@ -3113,21 +3139,21 @@
       <c r="K33" s="14"/>
       <c r="L33" s="14"/>
     </row>
-    <row r="34" spans="1:12" s="35" customFormat="1">
-      <c r="A34" s="34" t="s">
+    <row r="34" spans="1:12" s="25" customFormat="1">
+      <c r="A34" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34"/>
-      <c r="L34" s="34"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="14"/>
@@ -3187,6 +3213,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="A13:L13"/>
     <mergeCell ref="A5:L5"/>
     <mergeCell ref="F1:F2"/>
@@ -3203,10 +3233,6 @@
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3255,25 +3281,25 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="31" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="31" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="12" t="s">
@@ -3281,29 +3307,29 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
       <c r="C3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
       <c r="H3" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
       <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8">
@@ -3474,28 +3500,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="41" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="31" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="17" t="s">

</xml_diff>